<commit_message>
Update PI cardinality af9ee81eccb98f2aa82833f459653ccf02b1909f
</commit_message>
<xml_diff>
--- a/302-contenu-fhir---ajout-des-données-usager/ig/StructureDefinition-tddui-patient-ins.xlsx
+++ b/302-contenu-fhir---ajout-des-données-usager/ig/StructureDefinition-tddui-patient-ins.xlsx
@@ -60,7 +60,7 @@
     <t>Date</t>
   </si>
   <si>
-    <t>2025-07-28T14:46:36+00:00</t>
+    <t>2025-07-28T15:20:13+00:00</t>
   </si>
   <si>
     <t>Publisher</t>
@@ -11922,7 +11922,7 @@
         <v>79</v>
       </c>
       <c r="G76" t="s" s="2">
-        <v>80</v>
+        <v>89</v>
       </c>
       <c r="H76" t="s" s="2">
         <v>81</v>

</xml_diff>